<commit_message>
fix wording and text throughout improve docs
</commit_message>
<xml_diff>
--- a/data/demo/stressor_magnitude_demo.xlsx
+++ b/data/demo/stressor_magnitude_demo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbayly\Desktop\Projects\EN2691 CEPopMod\main\JoeModelCEShiny\data\demo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD64BEE2-DFD6-4A12-BE57-27DE098096CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8BB7376-96E0-476F-98C8-B1102966AFCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3348" yWindow="3336" windowWidth="15120" windowHeight="8700" xr2:uid="{5C00D94F-27E3-48C9-9AD6-363C8CBE8FED}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5C00D94F-27E3-48C9-9AD6-363C8CBE8FED}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -31,6 +31,133 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Matthew Bayly</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{B41EDCBB-C564-40B7-A62D-203B45B7E6EE}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>The HUC ID (or ID). This ID field must match the feature column HUC_ID in the watersheds spatial file.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{4A8F0528-C5B7-4C84-A297-813CF0B19615}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>The NAME of the polygon in the watersheds spatial file. This field must match the NAME column in the watersheds spatial file.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{1CF770B1-D091-407B-A19F-B4BD7A76B300}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Stressor Name. This must match information and sheet names in the stressor response workbook.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{BD681063-B2DF-4360-BFC4-2D05F6EA6F5F}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Stressor Name. This must match information and sheet names in the stressor response workbook.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{8B6907A1-472B-4B30-ACCE-A23DBB508625}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Mean value of the stressor in the given HUC (polygon).</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{E6E78B80-4519-4E1A-A05E-654DC48ED760}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Standard deviation (SD) of stressor values for the target HUC. Note that stressor values for each HUC are resampled in the simulation from a distribution with mean and SD values. Setting the SD to zero means that there will be no variability for the stressor value in the simulation.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{92667383-7FC4-42EB-A2F4-F385606ED6B2}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Type of distribution to use for resampling. Either “normal” or “lognormal”. We recommend using a “normal” distribution where possible. Testing coverage is incomplete for “lognormal”</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{E1B2B2DC-3ACF-4A72-8602-3A330D3D17EF}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Lower limit for resampling</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{19BDC1AB-4F65-43B8-8CD1-11F3F8261CF5}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Upper limit for resampling</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -430,13 +557,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -774,16 +907,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22C609AE-8BD9-48E7-939C-FB31F12B168F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22C609AE-8BD9-48E7-939C-FB31F12B168F}">
   <dimension ref="A1:J1649"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.109375" customWidth="1"/>
+    <col min="1" max="1" width="16.21875" customWidth="1"/>
+    <col min="2" max="2" width="23.21875" customWidth="1"/>
     <col min="10" max="10" width="10.88671875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -48613,5 +48747,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>